<commit_message>
Get daily reddit data: Tue Nov 19 08:11:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C472"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2913 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1gurymh</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>New to gel x</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouarw7ofbt1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1gurxhq</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>My first attempt at amethyst gemstone nails!</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gurxhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1gurwge</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>nail time is me time</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gurwge</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1guqxht</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>It’s hard to be in- love with something that also makes you feel so much self loathing 💪🏼</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guqxht</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1guqex4</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Would you buy these press ons?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfpejg93ss1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1guprwq</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic with a twist </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guprwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1gun1na</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Tips for a split nail?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk39l6qpur1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1gumwzi</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>How do you find an independent nail tech? I look on IG but it’s hard to find specific locations.</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gumwzi/how_do_you_find_an_independent_nail_tech_i_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1guluy3</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guluy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1gupagw</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Saw a post and had to get it!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpkmmra6gs1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1gup9al</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Builder Gel Extensions with regular nail polish on top</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gup9al</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1guoxh9</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Brown plaid for fall 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guoxh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1guoctl</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Rubber base gel</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1guoctl/rubber_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1guo0mo</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I really love the sparkling💖</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kceys1xs3s1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1gunmoc</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>need this in every color of the rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gunmoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1gunl8r</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">♥️forever a press on girly </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsctem2pzr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1gune3d</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Jelly Nails 😍</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7qc5h9vxr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1gujkso</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My autumn/thanksgiving inspired manicure 💅 </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1sy30ns0r1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1gumw2k</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Trying to remember indie brand</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gumw2k/trying_to_remember_indie_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1gumngg</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Vegas nails</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gumngg/vegas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1gulj7n</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Looking a daylight light to do my nails under - UK</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gulj7n/looking_a_daylight_light_to_do_my_nails_under_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1guk1tx</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Tile and glass nails</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/futjh4kk4r1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1gujuw5</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>smth for fall</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gujuw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1gujrvm</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>A set of press ons i made. This length is not for me 😆</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gujrvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1gujf9o</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Press ons 🥀⛓️‍💥</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gujf9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1guj8xs</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Current set!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ov47d76yq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1guj540</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2dqj3nbxq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1guiwxk</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made my own press ons for the first time. Hoping they last! </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guiwxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1guiknv</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Glamermaid vs Kiss vs. Red Aspen</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1guiknv/glamermaid_vs_kiss_vs_red_aspen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1guie96</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure 💅 </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guie96</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1guibge</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Lavender glitter!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guibge</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1gui3rw</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gui3rw/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1gui0l5</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>3rd fill in I've done!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmxgt42hoq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1guhvnx</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Favorite fall mauve 🍂</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul21k5eenq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1guho9p</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Black Matte!</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3eb378ptlq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1gued81</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Why do my almond nails tear on the side?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gued81</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1gugzxg</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Gel manicure help- What is this called and how can I ask my manicurist to fix her technique?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gugzxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1gug4zs</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Is this a concerning nail profile?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gug4zs</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1gudbfj</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Nail Strength</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gudbfj/nail_strength/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1guhlme</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>HELP W MT DAMAGED NAILS!</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp9dyal8lq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1guh3mc</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Happy happy</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guh3mc</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1guh0b3</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Blooming blues I just finished on myself</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guh0b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1gugoq1</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Action proud of them </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abdbkvrgeq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1guglhh</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Thoughts on Apex</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ax4z9gftdq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1gugbsb</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this new set! </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gugbsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1gufjcm</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Beautiful</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gufjcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1gufdku</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>How are the tips worn after 2 hours?!</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbive8tu4q1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1gufcb7</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>When you realize press on nails don't work for you</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gufcb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1gudwct</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Need some tips for diy gel overlay</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gudwct/need_some_tips_for_diy_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1gueoyk</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Some lil fall mushrooms</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gueoyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1gud1kd</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Just upgraded my e-file…wow!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gud1kd/just_upgraded_my_efilewow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1gucwl2</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Free edge lifting due to thin nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxuy0z2kmp1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1guctst</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Most recent nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guctst</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1gucqor</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>First acrylic set on myself since finishing school</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gucqor</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1gucphj</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Broken nail advice</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glgr7095lp1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1guclh3</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Frenchies</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrpwk92dkp1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1guckkk</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I don’t have dried flowers so I hand painted🙈 do you think I did good?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guckkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1guciw8</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Bonder recs, prep recs</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1guciw8/bonder_recs_prep_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1gub4uv</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Finished these just in time for a Christmas fair I have coming up 🫶</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gub4uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1guccsp</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>🎅🏻🎁</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2i6t02oip1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1gubiz4</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail stickers </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gubiz4/nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1gubi47</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Glamnetic nails no longer lasting me two weeks... let alone one! Anyone else?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gubi47/glamnetic_nails_no_longer_lasting_me_two_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1gubbti</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where are sassy saints made? </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gubbti/where_are_sassy_saints_made/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1gub8p7</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before &amp; After ( i do my own nails) </t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gub8p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1gub1j0</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>New nail set, but....</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gub1j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1gua5mo</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Problem with nail shaping</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gua5mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1gu9ix6</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Improper application or just fast nail growth?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu9ix6</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1gu9bks</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Any other glue I can use for press-on nails?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gu9bks/any_other_glue_i_can_use_for_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1gu98c2</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Game Day meant Nail Day. Hope Everyone Had A Good Weekend!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3l8x5a2wo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1gu9414</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>First attempt at a russian manicure 😊</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kqlvs2fvo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1gu8z49</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>What do you guys think of russian manicures?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gu8z49/what_do_you_guys_think_of_russian_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1gu7ndm</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Opinion on Sassy Saints powder manis?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gu7ndm/opinion_on_sassy_saints_powder_manis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1gu7urf</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I wished I asked for longer and sharper nails to make them more like silver claws, but I love the effect!!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu7urf</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1gu7qq3</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Little nails 😂🇦🇷</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6d8un4x9lo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1gu7pcb</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Cracked my natural nail in an awkward spot, what can I do?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ys1dzfzko1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1gu735k</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude Gel-X Classic Krispy Kreme </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny12pscago1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1gu6k2z</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I do acrylics on my regular nails? </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gu6k2z/should_i_do_acrylics_on_my_regular_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1gu6iei</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monthly Russian manicure </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my59jx8qbo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1gu6ezz</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They’re not perfect </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu6ezz</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1gu6cu1</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried something a little different </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orknditfao1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1gu2azn</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Nail glue advice</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gu2azn/nail_glue_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1gu5uyy</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>very basic but soooo adorable 🥰</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39wda3xe6o1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1gu5n9s</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Which style is better on me?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu5n9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1gu52ie</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>💙 Blue Christmas Nails 💙</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgsrm7atzn1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1gu4ss7</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Thoughts</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8y39trgxn1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1gu4loa</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>First mani in ages! Nail care tips needed~</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu4loa</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1gu3sor</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Fresh set with a new nail tech, does the colour suit me?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu3sor</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1gu3310</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do we think of cow nails </t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu3310</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1gu2svb</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>I love them!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prffie71dn1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1gu2owg</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>teal wt green aura 🩵💚</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu2owg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1gu15rf</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Gothic nails for the winters</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixklq8ryrm1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1gus5u9</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Tried my first Emily de Molly polish</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gus5u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1guryxw</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>I'm equal parts proud and horrified at my collection.</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz7lxlnkbt1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1guqrns</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Using press-on nails as a base for painting nails?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guqrns/using_presson_nails_as_a_base_for_painting_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1guphvp</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beyond polish - do they do black friday promotions? </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guphvp/beyond_polish_do_they_do_black_friday_promotions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1gup9uc</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting ready for Christmas </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gup9uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1guowil</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>ILNP Poison alternatives</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guowil/ilnp_poison_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1guolsa</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>My take on a downplayed mani</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mulgzrj9s1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1guoie9</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Builder Gel Recommendatioms</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guoie9/builder_gel_recommendatioms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1guo7k5</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Holographic powder recs?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc576dgp5s1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1guo52v</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Gel base coat</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guo52v/gel_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1gunjzt</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>initials on nails?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gunjzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1gun654</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>am I abandoning my fellow laqueristas by moving to false nails 😭</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gun654/am_i_abandoning_my_fellow_laqueristas_by_moving/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1gun2rb</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Season 2 Jinx nails </t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gun2rb</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1gums7m</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Go bowling, they said. It'll be fun, they said. They were wrong. </t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gums7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1gulkxf</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>How do you cope with having to go short? 🥲</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcpgtmbihr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1gul223</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>A perspective change that preserved my love of nail polish</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crpmoytycr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1gukszr</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>OPIxWicked Glinda the Good! &amp; Ga-Linda</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gukszr</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1gukrxs</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>I have brag on my teen for her skills!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gukrxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1gujxvq</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Cat sitting for my bestie and she told me to try her new polish. Thougts?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gujxvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1gujsyx</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Has anyone tried to Beetles lacquer? (Air dry formula, NOT the gel)</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gujsyx/has_anyone_tried_to_beetles_lacquer_air_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1gujghq</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>BIAB</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gujghq/biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1gui6ik</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any guesses as to what this color is? </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1z28dnopq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1gui5ra</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beaux Reves The Little Prince </t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jhdbjojjpq1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1guhvb9</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Pahlish Oozeling - super yellow?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guhvb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1guhlw4</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New fav </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guhlw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1guhezj</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Defended my dissertation with 'Cyantific' and 'I'm a Nerd' 😁</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guhezj</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1gugv6t</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Unearthed Heavy Metal</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gugv6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1gugh7n</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second time doing my nails! </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utnxdq6ycq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1gug2xn</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Help me choose BAE vs Halo</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gug2xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1guftk0</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Well Goodbye Paycheck...</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guftk0/well_goodbye_paycheck/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1gufr1w</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Sheer polishes reccs?</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fg62ob0l7q1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1guet21</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>House of Hades makes the rest of my life look dull in comparison</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d3kwolk0q1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1gueppv</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Autumn temperature shift</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gueppv</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1guep5r</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you mix regular nail polish (creme) with a topcoat to make it appear more like a jelly/more sheer? </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guep5r/can_you_mix_regular_nail_polish_creme_with_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1guecag</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>you're a JINX (but make it holo!)</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guecag</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1gud83o</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Moody fall vibes</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46x4mpbvop1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1gud2vz</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Will PPU orders deliver before Thanksgiving?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gud2vz/will_ppu_orders_deliver_before_thanksgiving/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1gucdal</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Shrinkage ?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gucdal/shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1guc3yo</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m still disappointed that Tactical Assault Possum arrived without a single weaponized possum, but I’m still down with the polish. </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4d9bg2hwgp1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1gubmqy</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Favorite Fall Mauve!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqdwh89hdp1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1guai7f</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Tried layering for the first time :) some fall leaves nail vibes 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guai7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1gu9ug6</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PSA: It’s Showtime from BKL is an absolute stunner, and it’s coming back this month </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxwf0teo0p1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1gu9k77</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>My wedding nails matched my henna!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3qum36jyo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1gu9jm7</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>attempted Fire nails</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu9jm7/attempted_fire_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1gu97yz</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Magnets to strongly magnetize Clionadh Psilocybin</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu97yz/magnets_to_strongly_magnetize_clionadh_psilocybin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1gu52gi</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>My fav go-to polish✨️</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og0h4psszn1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1gu7qg0</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Does anyone have comparisons for the following red magnetics?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu7qg0/does_anyone_have_comparisons_for_the_following/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1gu7nbw</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>LF&gt; BRIGHT light blue cremes</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu7nbw/lf_bright_light_blue_cremes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1gu6zut</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>My $4 mani 💚</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tll2bs2kfo1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1gu6tnf</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Last Magnetic from ILNP</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu6tnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1gu6aid</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Help with my garbage nails</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu6aid</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1gu5te5</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Any experience with dollar store top coats?</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu5te5</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1gu4xzw</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the village chief </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu4xzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1gu4iow</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Does Bunny approve of the mani?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu4iow</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1gu4fht</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Sea green over black</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu4fht</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1gu4fab</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Recs for pinkish red with strong yellow/gold shimmer?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu4fab/recs_for_pinkish_red_with_strong_yellowgold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1gu43q5</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>This is Some Boo-Sheet</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu43q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1gu3u74</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>How much do you spend on nail polish?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu3u74/how_much_do_you_spend_on_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1gu2r5m</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Remover of choice?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu2r5m/remover_of_choice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1gthsyo</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Favorite Multichromes?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gthsyo/favorite_multichromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1gto4ee</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>ILNP Poison</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a2mnq1lo4j1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1gtshca</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Attempt to do the viral red glasslike nails?? </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hfsisnwq4k1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1gu28wf</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gu28wf/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1gu1qpq</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Opinions on the purple to green multi-chrome polishes?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu1qpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1gu1foa</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Did a matte skittle mani for a Pokémon Go event this weekend.</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu1foa</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1gu10so</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Late night celestial manicure✨</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gu10so</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1gur82u</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Hi just want some feedback on these</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzy5dlhn1t1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1gupc7o</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Simple &amp; cute</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a84ptz1ogs1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1gunbqp</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Maritime Art .. Love the Lighthouse..</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hvlydkaxr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1gum6uq</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nailed the Christmas vibes! 🎄💅 </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gum6uq/nailed_the_christmas_vibes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1gul40l</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A close up of my new set </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w8nrm0gdr1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1gukd9e</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First winter set! </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gukd9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1guh8og</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Is christmas time on my nials</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2ghfe7kiq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1gugyoy</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This set I just finished on myself. Blooming blues. </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gugyoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1gugmb4</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>First time posting cause I am actually really proud of them</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5drinhozdq1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1guggee</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Love love love these 😭😭</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guggee</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1guf6qi</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Finished this set in time for a Christmas fair I have coming up</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guf6qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1gue64u</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Glues?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqw622cuvp1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1gu523h</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>💙 Blue Christmas Nails 💙</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thzpi8upzn1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1gu1szv</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Cowgirl nails:)</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwzmd8zn0n1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 20 08:11:17 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C472"/>
+  <dimension ref="A1:C641"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8457,6 +8457,2879 @@
         </is>
       </c>
     </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1gvklr4</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">white on white? </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw21ygdpj02e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1gvkffd</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>What builder gel should I use?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvkffd/what_builder_gel_should_i_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1gvjnmw</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Natural or acrylics? 💅</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvjnmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1gvjef1</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Second set I do on myself. Started learning about a month ago</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcmejzc5402e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1gvj5ev</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>🖤 Flirty Leopard 🖤</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvj5ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1gvimxx</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they’re so cute!! </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvimxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1gvimm0</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>How To Ask For a Refund?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvimm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1gvimd8</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>How To Ask For a Refund?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvimd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1gvij4x</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Feet so pretty 😍 </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61ryu3u6uz1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1gviiev</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i love my swatch sticks! </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgmhvnjytz1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1gvia6i</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Feelin’ Blue</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/877kaq4irz1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1gvh9zm</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Everything but the kitchen sink</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvh9zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1gvgjwd</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Painting the next nail on my Jinx Nail set. It's been 5 hours 😭 I'm nowhere near done 🥲🙏🏼</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl1vq6f3az1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1gvggcu</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvggcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1gvg6jq</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Embroidery design inspired nails</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3ethkbl6z1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1gvg3fn</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>What shape would you call this?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vr7nx93s5z1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1gvg4ql</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">finally went natural </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvg4ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1gvg4m5</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">finally went natural </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvg4m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1gvfz45</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tried red </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvfz45</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1gvfpur</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfhhfjqb2z1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1gvfpnv</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Gift Help for GF!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvfpnv/gift_help_for_gf/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1gvdcx4</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>i hated everything about these nails but they’re growing on me</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvdcx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1gvfaih</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Burberry Inspired Nail Set</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3d8koweyy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1gvew2h</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel polish recs! </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvew2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1gvevtg</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Do you like this color? I made them myself to a friend</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pen63zspuy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1gvdg20</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can never go wrong with a classic french! </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el3qmdg6iy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1gvd5px</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Best nail gel set for home use?</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvd5px/best_nail_gel_set_for_home_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1gvd3w4</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>What do you think of these french? ❤</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvtjzvxbfy1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1gvbk9r</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glowy nails for a rainy day 🌧️ </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5bmvldl2y1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1gvb9zs</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Feeling fierce with these new nails.</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epn8tiizzx1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1gvahyz</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Very basic question</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvahyz/very_basic_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1gva54t</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>DIY Dip and gel</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flvhry0frx1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1gv9lvb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Tried gray for something a little different. I think I like them lol</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59zkfcqcnx1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1gv9kzk</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Went with lightning nails this time! ⚡️⚡️</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv9kzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1gv9b91</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>My nailsss</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i3yhc866lx1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1gv8wee</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I want to buy my wife a Christmas gift but need help </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv8wee/i_want_to_buy_my_wife_a_christmas_gift_but_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1gv7r1a</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Did the TikTok nails because I’m basic AF</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqtgq50h9x1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1gv7eq9</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>newest press-ons ❣️</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv7eq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1gv4vbl</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>First time having my nails this long, hoping to grow longer.</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv4vbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1gv6uok</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top Coat recommendations </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv6uok/top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1gv50wj</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eras tour nails!! </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06oifh01pw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1gv6l27</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Cherry nails never fail</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy9gsr8o0x1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1gv5pjz</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>November nails</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2kteox5uw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1gv5mst</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Silky cat eye gel help?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv5mst/silky_cat_eye_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1gv5i1c</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>freshly made 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4hic0jisw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1gv5bbk</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>70s-ish Retro Nails :)</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv5bbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1gv59kf</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>First Holiday Set</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9wtehdnqw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1gv513n</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>My nails broke after 3 weeks</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv513n</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1gv4ybe</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Working on painting with my non dominant hand</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otiujorjow1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1gv4jbq</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Tips for cracks/repairs?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5c80luahlw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1gv3w0y</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Advice for a beginner who wants to start doing nails.</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv3w0y/advice_for_a_beginner_who_wants_to_start_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1gv3p5f</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Whats the best blooming gel?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv3p5f/whats_the_best_blooming_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1gv3ojv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Feeling Blue 💙</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv31r2lcfw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1gv2jpn</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Every time I use press on nails they end up breaking like this, any advice on how to prevent it? </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cn9h5pw67w1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1gv1a0h</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Tell Me Your Signature Nail Look</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gv1a0h/tell_me_your_signature_nail_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1gv2aj8</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What can I do to make my nail polish last longer? </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv2aj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1gv1eqv</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi everyone. I’m looking to gift my girlfriend one of these for Christmas and idk where to get one or recommendations </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjxcza0zyv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1guyf1j</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>This combo is so soothing to me, I can’t stop looking. Neutral/coffee inspired</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnq6f87bcv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1gv0w9c</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Autumn butterfly set - matched mani pedi</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv0w9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1gv0gi2</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Simple DIY Gel Nails</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gti3gob2sv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1guujuz</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Nail tech RED flags. What would you do?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1guujuz/nail_tech_red_flags_what_would_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1gv02d9</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arcane nail art (hand painted) </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl4qzhy3pv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1guzlzu</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Do You like or is dark?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y9vpilmlv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1guz076</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>🐻 Danish Cartoon ‘Rasmus Klump’ Nails 🐻</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plrh0a21hv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1guyvgs</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv8siz0yfv1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1guyv7h</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My fave sets of this year! </t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go9e61iwfv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1guyd8u</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Anyone else love seeing how sparkly their nails look in the sun?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guyd8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1guyaz7</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall brown </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sug52w4cbv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1guy9wm</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>11 Elegant Christmas Nail Design Ideas For The Festive Season 2024 – Maniology</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://maniology.com/blogs/maniology-blog/christmas-nails-art-design-ideas</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1guxi4e</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Love is Sharper Than Any Stake ❤️🔪🩸</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guxi4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1guxio1</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with how they turned out. </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xccz659u4v1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1gux60i</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>How often? Pls help me</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gux60i/how_often_pls_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1guwtah</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Learning to get my nails done 23M</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c63uky2nyu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1guwpgl</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Polygel Problems</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1guwpgl/polygel_problems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1guwjfs</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Guy here. 🫣 Pink gloss 🩷 Done myself 😋</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co0xfkh7wu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1guwel3</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Are my Nials long enough to get gel nials??</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrbpn46tuu1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1guwd97</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Does it look cute on me?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibgb3d26uu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1guvdty</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Do you like my press-ons?  I have reused them at least twice, which is why they look a little battered, but other than that, what would be your remarks?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guvdty</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1guvax4</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Cherry Blossom nails🌸</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1a5g6pdju1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1guuszk</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Do they look boring?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9e3cj6hdu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1guu49b</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>70s retro fall nails I did myself with my nondominant hand. It took forever but is so worth it</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guu49b</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1gut9j5</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Press ons 🫶🥰</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8bfahphtt1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1gut8g7</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BIAB for Vegas </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myfw19m2tt1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1gut0tt</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gut0tt/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1gvjnvp</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat recommendations </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvjnvp/top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1gvjkk1</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>My before and after…</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvjkk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1gvgh88</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co Butterfly Nebula 🦋✨🐸</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvgh88</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1gvf6hd</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Not my post/nails but had to share lol</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9z0el0fxy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1gvenih</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>holo taco wide brushes</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvenih/holo_taco_wide_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1gvehn1</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Unique mainstream shades?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvehn1/unique_mainstream_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1gvdpqg</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>ILNP - Canadian Shipping</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvdpqg/ilnp_canadian_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1gvdmpf</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Xmas For My SO</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvdmpf/xmas_for_my_so/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1gvdh0y</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Let Me Entertain You</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aol191ifiy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1gvdcin</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Base Coat/Remover issues??</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvdcin</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1gvcxjr</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Flakie skittle!</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ou4650bdy1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1gvcqkc</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for mooncat dupes </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvcqkc/looking_for_mooncat_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1gvcgvb</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>OPI Como Se Llama vs. Can't Read Without My Lipstick?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvcgvb/opi_como_se_llama_vs_cant_read_without_my_lipstick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1gvcc7e</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rant on misleading reviews/swatches </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvcc7e/rant_on_misleading_reviewsswatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1gvc9ek</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Let it GLOW</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvc9ek/let_it_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1gvc5ey</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>She’s so shinyyy</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvc5ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1gvbxed</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>ILNP - pyro</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvbxed</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1gvbopu</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Nails matched my drink today!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar0oqxjf3y1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1gvb89d</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this shade, so glowy and ethereal ☁️ </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/659kt6fzzx1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1gvapl1</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>My second time using poly gel!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zpmcq7tvx1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1gvahwk</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Fairy Dust in different lighting compared. Lighting is so important. </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvahwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1gvah4n</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Wow! 12 year old magnetic nail polish still works!</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvah4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1gvah0a</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>opi witch o’clock issues</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztsg1091ux1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1gvaffr</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In honor of my favorite writer releasing a new book today: </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvaffr</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1gva1fm</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Brand spanking new to painting my nails after biting them for years and need advice</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gva1fm/brand_spanking_new_to_painting_my_nails_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1gv9a3g</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Sudden, severe top coat shrinkage… can a higher altitude and/or lower temp environment cause this?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/box99gzxkx1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1gv8uk1</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i’ve been loving thermals lately! </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv8uk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1gv8lqq</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Witchy in the woods</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6yfcynopfx1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1gv781y</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Question for my chrome girlies</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tuw38hh5x1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1gv6wnc</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>finally painted all my swatches from my lil collection</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxgqfod33x1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1gv6nk9</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Everything about this color is so me! </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv6nk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1gv6gus</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Is nail strengthener supposed to just... Peel off?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gv6gus/is_nail_strengthener_supposed_to_just_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1gv61pv</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>ILNP is going to start selling 30lb horseshoe magnets!!</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xs6ghzljww1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1gv5dev</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I think I’m obsessed with magnetics 🥰</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv5dev</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1gv4sbq</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>This is a first for me!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbd4m0abnw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1gv4ese</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Thoughts on my Emily De Molly BF cart?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i0fevtkkw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1gv3u1i</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers - Infinite Nebula (solar/thermal) on extra short nails</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivofeghfgw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1gv3j2w</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Mooncat Reward: Strangeberry</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrrg5y09ew1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1gv3izd</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Bombshell</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv3izd</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1gv3b8e</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Your Heart's a Black Hole vs Poison? </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gv3b8e/your_hearts_a_black_hole_vs_poison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1gv37fn</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Fake Halo is stunning</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv37fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1gv31xp</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>My Clionadh Slickadelics came</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv31xp</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1gv2zie</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Trying a New Nail Shape!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zle1iedaw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1gv2dx0</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>✨ Naked or Not, (I) Told the Northern Lights to Keep Shining ✨</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv2dx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1gv25xn</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>It's so glowy 😍</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv25xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1gv1bbj</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Admitted to labor and delivery to have my baby and I can’t stop staring at my own nails 🤣</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv1bbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1gv0upr</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Got distracted!</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2nviykxuv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1gv0j4t</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Will my dip still last if I ask my nail artist to not file my nail beds?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gv0j4t/will_my_dip_still_last_if_i_ask_my_nail_artist_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1gv01fh</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR}Sassy Sauce Thanksgiving Skittle 🍂✨ </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv01fh</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1guzkv8</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>I'm slowly getting better at painting my non dominant hand😅</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3mzegkelv1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1guz2hh</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>When your nails match the ✨️ poop bag ✨️</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guz2hh</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1guyocr</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Cozy Fall 🍁</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny8k0utcev1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1guy76s</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y6zq32chav1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1guy73i</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Comparison swatches: ILNP Ruby vs Mooncat The Arsonist?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guy73i/comparison_swatches_ilnp_ruby_vs_mooncat_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1guy66x</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cards and Coins </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guy66x</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1guy5lo</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Let me see your storage solutions!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guy5lo/let_me_see_your_storage_solutions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1guy258</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>💚Elphaba💚</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guy258</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1guxrcw</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baeocystin on a chilly November day </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xc7g2sfw6v1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1guximx</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I’m in love 😍</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb5381pt4v1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1guxgy3</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Love is Sharper Than Any Stake ❤️🔪🩸</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guxgy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1guxbrp</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Labradorite by Dany Vianna is now restocked and being shipped!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1guxbrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1guxaaz</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">soft purple nails </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swagedat2v1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1guwlkt</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Super proud of these 🥲</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwxyccqpwu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1guevml</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>In search of a flaky topper</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guevml/in_search_of_a_flaky_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1gugjjm</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>New to Long-ish Nails</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gugjjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1gvjncf</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need some inspiration with ideas </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0qy1kp9702e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1gvira2</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Thanksgiving set</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvira2</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1gvidoh</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Last fall set ✨🍂</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vi9q1dhksz1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1gvgk6t</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Painting the next nail on my Jinx Nail set. It's been 5 hours 😭 I'm nowhere near done 🥲🙏🏼</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd09rn46az1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1gvfgtv</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked, the movie nail art inspo </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gvfgtv/wicked_the_movie_nail_art_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1gv7leq</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Washing brushes</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gv7leq/washing_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1gv6yx0</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Top coat</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gv6yx0/top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1gv6bhe</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Brown nails 🤎</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv6bhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1gv6907</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>First Holiday Set</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aizqulv6yw1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1gv3vtc</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Fall ombre</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7qlsvhsgw1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1gv3nto</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>My nails and my favorite perfume</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88dq2057fw1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1gv1kd4</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Disney Dreamlight valley nail art</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv1kd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1gv0xia</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Autumn butterfly set - mstched mani pedi</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gv0xia</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1guzo5u</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I love this design</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omryqf93mv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1guyzkh</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>🐻 Danish Cartoon ‘Rasmus Klump’ Nails 🐻</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow93qp0wgv1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1guxv27</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails for today </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilc83pkn7v1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1guuq65</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>What about them? 🤗</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uclvjgicu1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1gusyj0</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>My Poly Gel Marble French Nails😁</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gusyj0/my_poly_gel_marble_french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1gu9bnd</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'll keep improving </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soeptd2ywo1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1gu95mp</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner character nail art </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rduouyqvo1e1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 21 08:11:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C641"/>
+  <dimension ref="A1:C799"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11330,6 +11330,2692 @@
         </is>
       </c>
     </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1gway1m</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Nail strengthener on bottom of nails?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gway1m/nail_strengthener_on_bottom_of_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1gwax37</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Am I overthinking it</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwax37</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1gwadb9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will BIAB damage my natural nails? </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2jo4q8nd72e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1gwa0br</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Too soon? 🎅🏻</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyv2y7ge972e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1gw9x88</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>nail drawing</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0bmnlcd872e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1gw9qoa</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>first time trying floral 🌸</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsjh7ph7672e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1gw9fvd</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Wicked 💚🩷 French what do u think?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw9fvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1gw93v2</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>My nails never stay on when I do them myself.</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw93v2/my_nails_never_stay_on_when_i_do_them_myself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1gw8v15</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>switched to gel-x</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aftxr6zkw62e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1gw8q2f</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye nails with bows </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw8q2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1gw7knn</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Fall Nails🍂</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10zpatujj62e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1gw7g4v</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby's first press on set. </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw7g4v/babys_first_press_on_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1gw78u8</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>What do you think of this color?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5z6qzcacg62e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1gw6zx6</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out my Christmas designs! </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i1ibsj2e62e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1gw6xgo</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Tips for nail art on natural nails</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw6xgo/tips_for_nail_art_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1gw6zq2</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>First time trying almond shape! Not sure what I think?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw6zq2/first_time_trying_almond_shape_not_sure_what_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1gw6xd7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Last three sets I’ve gotten 😍 (oldest to latest)</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw6xd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1gw5pqf</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Blues” </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw5pqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1gw674o</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Are there any non-feminine nail color press-ons for guys?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw674o/are_there_any_nonfeminine_nail_color_pressons_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1gw5zus</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My Christmas bow nails🧣✨</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw5zus</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1gw5uks</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favourite set </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glmicbao362e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1gw5riz</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I have finally finished the second nail for my Arcane Jinx nail set! 🫠🫶🏼💙</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3krybuyx262e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1gw5m7j</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shipping this set to a friend </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke6q1r5o162e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1gw4nwk</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Festive Manicure 💅🏼✨</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsz9jvant52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1gw47pc</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best way to minimise damage when removing gel? </t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q63czo3up52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1gw56mg</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>My boyfriend and I’s 11 year anniversary is soon so I went with our favorite colors 🩶💜</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw56mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1gw53ey</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Doing these took years off of my life but I think they were worth it.</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pr8l3eb8x52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1gw50lh</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Twinkle Christmas Nails!!!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dcrvlifw52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1gw4q6q</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Still playing with green cat eye 💚</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rfygkym5u52e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1gw4aqq</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw4aqq/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1gw419n</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Idk what you call this style but I love these so much</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw419n</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1gw2tul</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Matching nails 🖤</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw2tul</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1gw2tse</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Work done for me </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa87lhtge52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1gw2qlc</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Love this take on a pink and white</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e9fy1oqd52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1gw1q8e</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue for gems that doesn’t require LED cure? </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gw1q8e/glue_for_gems_that_doesnt_require_led_cure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1gw1jes</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Low key thrilled with these press-ons</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdium9h5352e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1gw1l1b</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Strawberry Nails!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vny9n3m352e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1gw1cof</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Red and Blue Ombré</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo5byx64152e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1gw14uo</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Delicate or simple? </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrcqhc1ry42e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1gw0zif</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute and simple </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nz1xcjerw42e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1gw0smn</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got a fill and kept the bow on, I tried to soak the nail off with acetone for 40 minutes then my cosmetology teacher tried to use a clipper around the bow but the bow acrylic is really stuck to my nail :( advice </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw0smn</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1gw0sj4</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got a fill and kept the bow on, I tried to soak the nail off with acetone for 40 minutes then my cosmetology teacher tried to use a clipper around the bow but the bow acrylic is really stuck to my nail :( advice </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw0sj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1gw0av4</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Cozy Autumn Vibes 🍁</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cbyuggwm42e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1gw05j6</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k7up6ivhl42e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1gvzfxd</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Red Cateye Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvzfxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1gvytkx</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Best products for making nails stronger?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvytkx/best_products_for_making_nails_stronger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1gvydnz</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark berry gel manicure for fall! </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvydnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1gvybdv</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>I think I’m done</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlt0ed8l142e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1gvxoqr</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my first two sets, not bad </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxoqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1gvxl4u</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh acrylics! </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxl4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1gvxehg</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>my bare nails :3</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxehg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1gvxbtz</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Nail growth progress</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91iy7vkdu32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1gvx23c</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time press on nails  - Are they looking ok? I have very short nail beds, as I bite my nails </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvx23c</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1gvwxbl</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue on nails </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvwxbl/glue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1gvw7z1</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best press on nails for wedding? </t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvw7z1/best_press_on_nails_for_wedding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1gvw77a</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>First full manicure I’ve ever done!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yybtnw59m32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1gvw0hy</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Nail Art Dump💅</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvw0hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1gvvnel</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>G59 and twenty one pilots sets i was commisioned💀😵❌✝️</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvvnel</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1gvvgwy</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almost one year of making my own press-ons - thoughts on some of my favorites? </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvvgwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1gvv6k4</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>nailsss update 💅💋❤️😇🥰 extra special cuz I’m a nail biterrr 🤭</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pkqlczwte32e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1gvv6ec</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>I’ve got my nail broken vertically, anyone know how to fix it?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sadcmz4re32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1gvv600</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Rave set i just shipped out !¡!🕺</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvv600</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1gvu6sp</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Woke up to my pinky nail broken off 😿💔</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvu6sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1gvu1co</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Cherry nails for a friend🍒</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxuurp1l632e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1gvhbve</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Can I put nail extensions over a green nail?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bb1d5qohz1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1gvtwny</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Tried to do the smoke effect. Can say I'm pleased even if it doesn't look like smoke</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktvlvxfo532e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1gvrkcc</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some tangled inspired shorties for my Disney trip this weekend! </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qirtzyvrn22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1gvtjhl</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Any tips to prevent this?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/im69ei5z232e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1gvsuz2</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I'm Absolutely Devastated - Need Press On Tips</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvsuz2/im_absolutely_devastated_need_press_on_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1gvsw86</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Builder gel journey (Sep 5- Current Day)</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvsw86</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1gvsv7i</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guestion about the quantity of gel/acrylic </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvsv7i/guestion_about_the_quantity_of_gelacrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1gvsdyk</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>💙 Avatar Nails I did recently 💙</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvsdyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1gvp9re</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>The execution vs the inspo</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvp9re</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1gvs1kw</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Are these press ons ok or do they look horrible?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lajfoejr22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1gvroe7</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love green colour and short nails </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr4syekoo22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1gvrnjx</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail elegance </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5e9im4io22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1gvqbqj</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>No winter blues here!</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zts9q0ld22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1gvq9uu</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>So…did I pass the exam?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87d53kv4d22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1gvmr7x</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dam Nail Polish - Thai and Stop Me </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvmr7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1gvm7rw</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn vibe </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5hvykbf612e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1gvm1du</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Soft floral glam 🌼✨</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn1etxw5412e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1gvlzzt</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>The 12 Days of Nailmas - Day 1</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vp0zrql312e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1gvlv4o</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>3D gel for depend up lamp?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvlv4o/3d_gel_for_depend_up_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1gviq2j</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Finally proud of my natural nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gviq2j/finally_proud_of_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1gvjlkz</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was looking for nail inspo but couldn’t find anything I liked so I came up with my own and I adore these nails! </t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i7wjyyvm602e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1gvih9l</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Hey, I’m trying to replace my sister’s nail polish but I don’t know what to get.</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gvih9l/hey_im_trying_to_replace_my_sisters_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1gwbbv5</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Nail polish won't come off. Send help</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwbbv5/nail_polish_wont_come_off_send_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1gwa14o</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Does anyone else have one of those plastic containers that store 48 bottles of polish?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwa14o/does_anyone_else_have_one_of_those_plastic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1gw9k0r</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>LynB “Good Scents of Humor”</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw9k0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1gw9i5d</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comparison pics of Polished for Days vs. KBshimmer </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw9i5d/comparison_pics_of_polished_for_days_vs_kbshimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1gw8kts</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Mundo de Uñas shipping times?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw8kts/mundo_de_uñas_shipping_times/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1gw8jtt</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Hunting For - NEONS &amp; PASTELS</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw8jtt/hunting_for_neons_pastels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1gw7uz2</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Latest mani done by myself at home! Details in post.</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fehwu7cm62e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1gw6yz1</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>KBshimmer swatch request!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw6yz1/kbshimmer_swatch_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1gw6tm8</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly Sandwich Skittle </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw6tm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1gw6d7y</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Damage coverage for my shorties</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1yhywxa862e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1gw4car</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Dots</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw4car</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1gw3lcu</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I able to file my nails into a rounded shape or are they permanently square? </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw3lcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1gw39uc</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Ooo look what i found.</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4izqlq4i52e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1gw38tf</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comparison request: ILNP Moondust vs. Sally Hansen Adrenaline Crush </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw38tf/comparison_request_ilnp_moondust_vs_sally_hansen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1gw38au</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First indie polish! Nice purple shimmer 💜💕</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw38au</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1gw2at0</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Magnetic acrylics 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xqqsqbe7a52e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1gw2aek</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Swatches looking like a lava lamp</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fen34umq952e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1gw21s2</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Does anyone want to talk me out of any of these while Reddit is still functioning for me? ☺️</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gw21s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1gw1v15</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Clown glitter</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw1v15/clown_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1gw11do</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>[Looking for recommendations] What are your favorite opalescent finish nail polishes?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw11do/looking_for_recommendations_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1gw0nxm</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>What the- Why- How- is my quick dry top coat peeling?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw0nxm/what_the_why_how_is_my_quick_dry_top_coat_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1gw0hu7</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>That shifty glow gets me every time</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/brel8b7eo42e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1gw0ia2</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Why is The Top to My Infinite Shine Polish Gold Instead of Silver</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt1yvfrso42e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1gw0g1p</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Top Coat Ruined my Cat Eye Effect?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw0g1p/top_coat_ruined_my_cat_eye_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1gvzri4</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I’m calling this one “the squiggly little lines my nerite snails leave on the glass of my shrimp tank” 〰️〰️〰️</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvzri4</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1gvzbws</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>The nail polish I've been looking for, for years!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvzbws</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1gvyyn4</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>My own galaxy to stare at all day ✨</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvyyn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1gvyr5c</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>I started collecting nail polish in September. Finally, a use for my label maker!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvyr5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1gvyl25</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>What shade is your soulmate??</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t0gw5jhi342e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1gvyiz3</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Opinions on G&amp;G and others</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvyiz3/opinions_on_gg_and_others/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1gvxwu5</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Pretty green for the Thanksgiving week into Christmas season</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6ry3q4ny32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1gvxwb6</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What HT Spyglass *should’ve* been. </t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxwb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1gvxt75</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The best dipping powder? </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvxt75/the_best_dipping_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1gvxhqn</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>ILNP chai latte; first time not going for a second coat</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxhqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1gvxawg</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>What do we think? 🍄‍🟫</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvxawg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1gvwzop</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Help with my nail shape?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvwzop</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1gvwzfv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI’s Got the Blues for Red surprisingly lifts my spirits </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvwzfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1gvvioe</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My second ILNP mani- Fairy Dust 🧚‍♂️ </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvvioe</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1gvvd7w</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unexpected new fav combo </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzzyprn7g32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1gvv6tv</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>My favorite polish is discontinued 💔</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvv6tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1gvus7c</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Found these in the collection. Not sure the shade name of the middle one</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af4lwy72c32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1gvuq06</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>F*ck These 273 Fish in Particular (pics in comments)</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tj9p97pmb32e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1gvtv2s</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Brand top coats</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvtv2s/brand_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1gvtuze</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Skittling through my untrieds</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvtuze</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1gvtbj4</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Quite Literally Dead Inside and God of Idiocy</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvtbj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1gvtb59</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>HELP WITH PRESS ON TIPS, IM DEVASTATED + A CAUTIONARY TALE</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvtb59/help_with_press_on_tips_im_devastated_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1gvsx1r</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>opi - cave the way</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zu8ha059y22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1gvstsf</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Flash-Ionista</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvstsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1gvs92v</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it's bordeaux weather </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvs92v/its_bordeaux_weather/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1gvrmqu</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Faces</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvrmqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1gvrldm</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Feeling fancy</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvrldm</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1gvrccf</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Winter is around the corner 😍💙💅</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvrccf</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1gvqv2l</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>OPI - My own bestie</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a8sjvjzh22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1gvqme1</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>That Other Girl</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvqhzw</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1gvqchm</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>my latest obsession: thermals!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvqchm</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1gvpwv9</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>🫧💖Glinda💖🫧</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvpwv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1gvohsx</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Trying something different with my usual June/Nov manicure’s accent nail. Results… mixed.</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ocajfhww12e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1gvnzkz</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>First snow of the season and I’m caught wearing Barbie pink</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvnzkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1gvnd0g</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>30lb magnet</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvnd0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1guxihf</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Blues and purples not vibrant enough -- is indie really going to help?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1guxihf/blues_and_purples_not_vibrant_enough_is_indie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1gvhwip</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lights Lacquer </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvhwip/lights_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1gvi7fy</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Help Please</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvi7fy/help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1gvj4lt</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>DND#429 Boston University Red</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gvj4lt/dnd429_boston_university_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1gvms3o</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dam Nail Polish - Thai and Stop Me </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvms3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1gw60dm</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>What do you think of my nails when they were short?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbib5ih1562e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1gw5ra1</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>I have finally finished the second nail for my Arcane Jinx nail set! 🫠🫶🏼💙</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey5qqcsv262e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1gw4yap</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Glitter Christmas Nails!!!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k7svpbyv52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1gw4wrp</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>My Marble French poly gel nail</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/936bulwkv52e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1gvwhde</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Holiday in Red!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqrksw4bo32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1gvv9ag</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Handcrafted by yours truly ✨💜</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvv9ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1gvsddi</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>💙 Avatar Nails I did recently 💙</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gvsddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1gvqzd0</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>I nailed it♥️</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c41tu15j22e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov 22 08:11:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C799"/>
+  <dimension ref="A1:C989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14016,6 +14016,3236 @@
         </is>
       </c>
     </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1gx2yrf</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>One of my first sets!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx2yrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1gx2oi7</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Colour recommendation?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwtq1oy6re2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1gx1y02</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails!! </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx1y02</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1gx1xmq</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>helpppp</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyk6kagihe2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1gwxegs</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Builder gel nails breaking…</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwxegs</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1gx11go</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Can you tell if they’re press-on’s?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx11go</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1gx084k</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Found these looks on Pinterest (@medastar, @My Eriksdotter). What kind of gel polishes should I buy to get this look? Very new to gel polishes so user-friendly options (if that's a thing?) would be appreciated!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx084k</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1gx0mbf</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Glue with stick on nails?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gx0mbf/glue_with_stick_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1gx0g29</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for at home gel manicures? </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gx0g29/advice_for_at_home_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1gx0dhc</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Did butterfly nails on myself this time 🦋</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q6gancqzd2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1gx031a</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She was a Fairy </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx031a</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1gx02vl</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Vacation nails ✅🌴🐚🌊</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l4jrbe8rwd2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1gx009l</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite design </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qbm86p1wd2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1gwzuzj</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pressies </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4t2tbelud2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1gwzbm0</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Sand colors, my favorites</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6169im6pd2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1gwyy0m</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">too early to get redone? </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00g2natgld2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1gwyxly</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Simple holiday nails</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee01210dld2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1gwyaz2</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Getting ready for Thanksgiving with Painted Polish Spill the Green Beans 🦃🍂🥧</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwyaz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1gwwuu6</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Hitchcock Nails</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwwuu6</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1gwxbck</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fill time </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwxbck</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1gwwvni</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall set 🤎 kitty approved </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ptpe7qc2d2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1gwwn6v</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>In honor of the F1 Las Vegas Grand Prix this weekend: Ferrari Red 🏎️❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwwn6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1gwwmse</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>gel on plane</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwwmse/gel_on_plane/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1gwufvc</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Dip powder anyone?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwufvc/dip_powder_anyone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1gwvc9g</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nails!! </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbsezmynoc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1gww4rv</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Love love loveeeee❤️</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gww4rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1gww3by</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Brown cat eye 🫶</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr1nfnj7vc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1gwvm3g</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here we come Toronto N6! </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwvm3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1gwvkgx</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>$90 for a FILL</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dxryk5nqc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1gwuabm</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Advice for timing etc</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rczxn4uufc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1gwucw0</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY Manon Blackbeak inspired nails. </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31r5pleegc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1gwuyys</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I’ve gotten </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwuyys</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1gwuxwb</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>I change my set every couple of days</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwuxwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1gwut54</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried to do some cat-themed nails on a whim, but i didn’t have any nail brushes and had to work with regular ones </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwut54</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1gwug34</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Anyone know some good nail polish brands? (In Australia)</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwug34/anyone_know_some_good_nail_polish_brands_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1gwtr3d</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>mermaid vibes 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h89v0uhbc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1gwt951</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 weeks grown out and still looking great </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8ccjnpg7c2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1gws309</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Help💔</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyi3bkr8yb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1gwsrs1</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Will polish remover remove cured gel?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwsrs1/will_polish_remover_remove_cured_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1gwsjwt</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I use acetone to "remove the treatment between applications"? </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwsjwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1gwsf2s</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love w these press ons </t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x84he6bu0c2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1gws0y9</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Cherry Chocolate 🍒</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaem620txb2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1gwrymo</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Best nail type?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwrymo</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1gwrvfi</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>my nails a fire! Do you like this design?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hkwjokfwb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1gwrpr9</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these myself! Christmas theme nails </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwrpr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1gwrja6</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>First time getting cat eye nails!</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwrja6</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1gwqz92</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>First time doing gel x</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwqz92</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1gwra24</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Went to remove shellacs and nailtech drilled out paper thin my natural nails... What should I do?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwra24</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1gwr8w8</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short but nice color option </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu4ujxaurb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1gwr5zv</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>My beautiful nails 💅</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqdnud38rb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1gwr3gu</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Think it is very delicate</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uqxxh7oqb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1gwpo9i</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>another victory against the nail biting monster</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwpo9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1gwq48x</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arthritis finger bumps, need advice </t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwq48x/arthritis_finger_bumps_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1gwq396</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wholesale supplies </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwq396/wholesale_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1gwq1jd</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>My birthday nails!</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swox738rib2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1gwq0rx</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Russian Almond shape achievable on natural nails??</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwq0rx/russian_almond_shape_achievable_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1gwplx2</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time and now addicted to chrome </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48zcffxjfb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1gwpb5r</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>I did these myself 🐝</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hp81xthcdb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1gwoxhz</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Would you rock this?😏</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2k1g5jkab2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1gwodgu</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Pokemon Nail!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwodgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1gwnrdh</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Green, but not too green</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/203su2xz1b2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1gwnmqn</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should cuticles sting after manicure? </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv17xo821b2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1gwn7sd</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Felt like something girly x</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hejgsmz4ya2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1gwn3dr</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Sweata weatha</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b7gzrw7xa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1gwms40</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Vermillion vampy</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwms40</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1gwmp5m</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Set ❄️ </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3qho5vmua2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1gwmhm1</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Another work from my cousin🤭</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h03kt9t5ta2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1gwmefa</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My sister (self taught) did my 💅I’m in love. What are some suggestions for next time?? </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gowmorjsa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1gwmdbm</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>My cousin makes these, I’m so proud of her</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjmu912csa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1gwm3cm</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Falling into press ons 🍂</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsu73mfeqa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1gwlvsj</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Thoughts ?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwlvsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1gwm2hj</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XL nail problems with piercings </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwm2hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1gwlkbw</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>my first ever set of nails</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyh3dbiqma2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1gwle0s</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Of course I broke my thumb nail immediately after painting them</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do20jguila2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1gwku6q</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Purple silver combo💜</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwku6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1gwksd1</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>2nd time doing gel nails myself 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zw22325hha2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1gwkpu1</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got a new manicure </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwkpu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1gwkeq8</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my nail biters…any advice for this bride to be? </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwkeq8/for_my_nail_bitersany_advice_for_this_bride_to_be/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1gwkdtn</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gold and bling! </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufvtmy4qea2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1gwk05v</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>My sister (self taught) did my 💅 I’m in love! Any suggestions for the next time??</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwk05v/my_sister_self_taught_did_my_im_in_love_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1gwjo9v</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>What is this? Is it normal</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2j3ksuq9a2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1gwjtkg</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Thanksgiving set 🤩</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwjtkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1gwjrxe</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Can’t quite catch the right lighting…</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cdzthfsgaa2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1gwaobk</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic Allergy </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwaobk/acrylic_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1gwbk32</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV pen burn? </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/402cg6q2t72e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1gwg3q7</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>As someone who pretty much only wears black, I like to let my nails be my color - done by @bellarose_nails on Instagram</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwg3q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1gwihb7</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Whimsigoth inspired nails by me 🔮</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icqcgcbv0a2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1gwikj0</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice on Gel X for beginner </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwikj0/advice_on_gel_x_for_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1gwidhv</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>When did it stop becoming common practice to clean up the cuticles?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwidhv/when_did_it_stop_becoming_common_practice_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1gwi81s</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>👸 Cinderella Disney Nails 👸</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwi81s</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1gwhw1u</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egqoee2po92e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1gwhtzc</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some nails I’ve done :) </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwhtzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1gwhf4p</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Self defense / sharpest nails? </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwhf4p/self_defense_sharpest_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1gwhdnt</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Should I keep up my acrylics?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwhdnt/should_i_keep_up_my_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1gwgorh</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>how harmful is acrylic in the process of growing out your natural nails?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8adwnnise92e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1gwglzz</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Teeny Snowflakes ❄️ 🎄</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5ex1b24e92e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1gwg5er</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Nail polish toppers over gold chrome on natural nails 💫</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwg5er</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1gwfyeb</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Shaping press-ons</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwfyeb/shaping_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1gwfgob</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>a russian manicure for my thanksgiving trip ✈️</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwfgob</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1gwdvi2</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Press on nails 💅</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1x4gag23n82e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1gx2vs9</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>It's incredibly shiny</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx2vs9</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1gx1fox</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>{PR} I’m Fun Sized by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx1fox</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1gx0veo</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Color Dupe</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1od6xl045e2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1gx0izj</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Deciding between ILNP Enchantment and Mooncat Weeping Willow</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gx0izj/deciding_between_ilnp_enchantment_and_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1gx0dk8</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Speechless over this Salon Perfect shimmer</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sugcy4crzd2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1gwzn1s</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Ulta Chic Peek</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ulta-chic-peek-2024-03iV7IV</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1gwza6y</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alright y’all pick my thanksgiving mani for me please! </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwza6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1gwz3et</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Cirque Points Rant</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwz3et/cirque_points_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1gwyhsm</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>ILNP Holographic topper question</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwyhsm/ilnp_holographic_topper_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1gwy9pj</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Getting ready for Thanksgiving with Painted Polish Spill the Green Beans 🦃🍂🥧</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwy9pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1gwxe4d</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>What should I get? Rogue vs Cupcake Polish</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwxe4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1gwwviz</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Is this the right one?!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xq7scn8b2d2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1gwwtfn</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>SIMPLY SHREEEIK (POWER IS BACK Aaaa 😆)</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3jlb86r1d2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1gwws59</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Jior Couture Replacement Brush?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iupbmpch1d2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1gwwj3q</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Why am I like this?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz3g87s8zc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1gww6w2</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kathleen &amp; Co formula? </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ldtlv74wc2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1gww06t</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Returning with my results after asking if I could mix topcoat or clear coat with cremes</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gww06t</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1gwvsvr</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>swatches for velveteen/cashmere - ilnp &amp; queen of the dead - mooncat next to each other?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwvsvr/swatches_for_velveteencashmere_ilnp_queen_of_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1gwvqgo</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Magnets</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwvqgo/magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1gwva6j</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know a similar shade to this? I can't find one </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3sbhlj5oc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1gwv9na</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wildflower Butterbean 🥰🧸 </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwv9na</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1gwv1bf</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>I bought new magnets and they're very strong...</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwv1bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1gwucna</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Mooncat - Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwucna</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1gwtw3c</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💙 Holo Taco Vitamin Glow - honest opinion </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwtw3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1gwtc3z</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Is this gel polish on skin ok?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ygkuck48c2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1gwtb8t</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Glitter patter✨️</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwtb8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1gwsuuz</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They’re supposed to be blueberries!🫐 </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwsuuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1gwro49</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for broken nail :( </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwro49</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1gwr7dq</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Earth To Gaia is simply beautiful </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwr7dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1gwqvyp</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Looking for Recs on Cuticle Nippers</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwqvyp/looking_for_recs_on_cuticle_nippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1gwq2vz</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clionadh Cosmetics - Dark 'N Stormy Golden Prairie </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwq2vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1gwpux7</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A little upgrade </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwpux7</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1gwpfpd</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Not sure about this one!! 🩷🩷</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pftpjkg9eb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1gwoqpe</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Any ideas on how to recreate this mani? Megan Thee Stallion's rocking it!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwoqpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1gwo89z</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Succulent Garden </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dvdvlri5b2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1gwo083</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell 🦋</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jlktwxbo3b2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1gwnyg9</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUGGESTIONS NEEDED </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwnyg9/suggestions_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1gwnox6</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Does anyone know of any polish/gel in these colors ??</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwnox6</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1gwnmpa</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Vitamin glow dupes?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwnmpa/vitamin_glow_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1gwn1ss</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Mooncat sale - what’s in your carts?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4alldsqxwa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1gwmw8j</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>🍁Autumn Ombré🍁</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwmw8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1gwmsru</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>And the award for worst time to break a nail…💍</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwmsru</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1gwmkw2</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Misty Question </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwmkw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1gwmhzo</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Comparing ILNP look alikes</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwmhzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1gwm9sb</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>OK so what are we doing for storage?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gr1fccnra2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1gwm76h</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>UnderGlow? More like UnderWHOA</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwm76h</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1gwltk9</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just love reflective glitter </t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6o96fdioa2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1gwlgie</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bombillate </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwlgie</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1gwlcly</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Anything repetitive in my ILNP and Mooncat carts?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwlcly</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1gwkz53</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Does anyone know of a similar polish?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n31b348ria2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1gwkd97</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish Names </t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwkd97/polish_names/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1gwk96k</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Skittle - Waiting for spring!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwk96k</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1gwjzew</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Stamping polish suggestions</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwjzew/stamping_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1gwjwm2</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When you introduce your two besties </t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwjwm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1gwj3fa</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>sagebrush🍃</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxvd69po5a2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1gwix79</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Nail Polish Advent Calendars</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwix79/nail_polish_advent_calendars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1gwioje</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Wrinkly fingers! Help!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9n2ek7p2a2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1gwimni</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Purple Flakie Ombré</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwyaa8lb2a2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1gwhvgt</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How to make my polish last at work?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwhvgt/how_to_make_my_polish_last_at_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1gwhfim</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Excuse the bubbles.. slowly working my way through BKL'S "The Craft" collection.</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwhfim</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1gwh3np</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Green and pink for Wicked 💚🩷</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwh3np</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1gwh2cf</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t xml:space="preserve">short nail art! </t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwh2cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1gwgtsu</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slick-a-delic more like Sick-a-delic Clionadh Cosmetics Norpsilocin </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwgtsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1gwenc0</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Feeling blue</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwenc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1gwe8se</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help: get rid of one polish from each photo? </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwe8se</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1gwe0ha</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>My first order is here!!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5x70n5to82e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1gwdnsn</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Convince me to try magnetics again</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm0w7k8lk82e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1gvvz9o</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Fall Wallpaper Asthetic</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo6zwp1nk32e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1gw0ayu</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails won’t take polish, please help! (Photo for example, so sorry for how gross they look) </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5mf28lxm42e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1gw74hx</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Mooncat Jewel Beetle v EDM Current Events comparison</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw74hx/mooncat_jewel_beetle_v_edm_current_events/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1gw7q5d</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Root of All Evil = Pixiedust over From the Ashes? Would it be remotely similar? </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gw7q5d/root_of_all_evil_pixiedust_over_from_the_ashes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1gwbvgu</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Regular top coat over gel polish for allergy prevention</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwbvgu/regular_top_coat_over_gel_polish_for_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1gx23nf</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake press on nails 🍓</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71ef3x5gje2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1gx01lf</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Vacation nails ✅🌴🐚🌊</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57m6756ewd2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1gwzdly</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Holiday Set ^-^ Blue Cornflower </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gwzdly/first_holiday_set_blue_cornflower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1gwvkxl</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Here we come Toronto N6!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwvkxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1gwvajb</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Crystals under Gel</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqosfbk8oc2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1gwutpz</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>I change my set every couple of days</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwutpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1gwup25</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My friend made me this beauty</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy2cpp36jc2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1gwtdge</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>New set 🍒🩶</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwtdge</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1gwsmbm</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Do you think i could start selling press on nails?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwsmbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1gwrhz6</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Wanted to show off my Wicked nails, but Boombox🐈‍⬛was hogging the best lighting!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwrhz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1gwrci2</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>We are on Christmas Eve</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vjkubhmsb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1gwq3fr</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice/opinions </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53fywra7jb2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1gwpu7v</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I love em🥰</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwpu7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1gwpr80</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Gingerbread Nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwpr80</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1gwmk6m</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on sets I made </t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lydw8xeota2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1gwlgzx</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Cherry nails! 🍒✨</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/antfwp93ma2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1gwk3qi</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Need help with a nail lover's gift? She's asking for gel polish.</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gwk3qi/need_help_with_a_nail_lovers_gift_shes_asking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1gwi7bp</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>👸 Cinderella disney nails 👸</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwi7bp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov 23 08:09:46 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C989"/>
+  <dimension ref="A1:C1203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17246,6 +17246,3645 @@
         </is>
       </c>
     </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1gxtkkm</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Grit on sanding bands</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxtkkm/grit_on_sanding_bands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1gxt7il</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink Blinged Set! 🤍🩷 </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxt7il</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1gxub8n</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Bubbles on nails</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxub8n/bubbles_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1gxrvcs</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Anxious about getting nails done. How do I get through the appointment?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxrvcs/anxious_about_getting_nails_done_how_do_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1gxsunn</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>i did my own nails (and my bf)</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxsunn</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1gxspom</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Still very much a beginner, but very proud!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyx6ws7sal2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1gxsoyp</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I had to cut my nails for paper writing season. </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxsoyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1gxs90g</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Press-ons</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxs90g</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1gxs78s</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>My little sister is spending the night. Of course we had to do some nails!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxs78s</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1gxs1gv</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Dip for Soft Nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxs1gv/dip_for_soft_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1gxrnl9</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Icy nails 🥶🩵💙😍 Fresh set!</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/258gshgdzk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1gxr04q</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Fall Set I did on myself today! </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t964bfvisk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1gxqpim</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>The latest set I did for the holidays 🌲</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhokl7gkpk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1gxqcfj</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Press on's I found at the mall</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz2guq6zlk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1gxqaf4</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>What do you think? Does that design suit me?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6b3jtp3lk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1gxpzr5</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Can I get some help please?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxpzr5/can_i_get_some_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1gxptrx</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>How much would this cost?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8exovkwvgk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1gxpajx</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Which nail lamp to invest in?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxpajx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1gxp5em</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails 1 inch minimum </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxp5em/nails_1_inch_minimum/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1gxoyw6</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>very demure</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgqobvsl8k2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1gxovjc</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tipex nail method question! </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b13n30rp7k2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1gxol2l</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple. Elegant. Obsessed. </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fllgpjr05k2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1gxo8ju</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Help - is this normal?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxo8ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1gxo6lc</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>New nails! The third set I’ve traded for baked goods!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxo6lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1gxjr04</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Which one is better for bridal nails?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qg75xxdl0j2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1gxnvyg</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>1 coat funny bunny 1 coat bubble bath gel x</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7vxbdgryj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1gxmtnm</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what can i do to make my hands to lengthier and more feminine </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxmtnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1gxn9o5</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Weird fingers! Nail shape advice </t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxn9o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1gxnryw</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails I trimmed </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxnryw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1gxnh5t</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Press ons ✨</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfb53ox6vj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1gxnebx</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Still learning to work with builder gel, I think this turned out pretty good.</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2n55iwcuj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1gxn5xx</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rubber base on natural nails </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxn5xx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1gxmuyf</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Gobble gobble🦃</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpe7ngvvpj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1gxmtab</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Help meee please</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61fmq9hhpj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1gxmi9e</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Fresh set! ♥️🍷</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vxlunqwmj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1gxmdap</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Tamagotchi nails!</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxmdap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1gxmc64</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>how do we feel about this color?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx8mqdgilj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1gxm1np</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>New Year’s party set 🎊</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxm1np</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1gxlsnr</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>What do you think? I love them.</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y8gaqd5hj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1gxl3ss</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for affordable builder’s gel </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxl3ss/looking_for_affordable_builders_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1gxkcyi</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>What’s the best way to remove only the color from my gel nails?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxkcyi/whats_the_best_way_to_remove_only_the_color_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1gxk7g0</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I like sheers over solids </t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxk7g0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1gxjflu</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxjflu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1gxiyny</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Russian mani?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxiyny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1gximdg</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Autumn boho set - matched mani pedi</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gximdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1gxi1cf</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Baccarat glass nails 🪩✨</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxi1cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1gxhfhy</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked nails </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qq1x2heii2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1gxgzle</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddu987hzei2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1gxgdxf</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Love these ❤️</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxgdxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1gxftoj</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Since it’s Wicked day, here are my Glinda and Elphaba inspired nails 💖💚 </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxftoj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1gxebh9</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Nail broke, what do I do?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trlagx2tuh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1gxecwy</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail indentation </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxecwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1gxedwm</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Vacation nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxedwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1gxg2cy</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>A holiday set I just made for a friend 🎅🏻🌲❄️</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p48imb7w7i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1gxg1wr</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Manicure</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nzj2cus7i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1gxg1fj</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need nail color recs! </t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8cecg4p7i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1gxfxlj</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So grown out, what’s your fav brand of dip powder? </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wgw9gow6i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1gxfsww</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>spent the whole night on these</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktaq30mx5i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1gxfmtf</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Finally found my shape</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mc4qwtn4i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1gxfeha</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Wicked nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxfeha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1gxfb0r</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>These were supposed to be “pink Christmas” but I got carried away 😆</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edintmg82i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1gxf3bs</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>☀️🐚🪼🌊</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjr7684n0i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1gxenlp</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>I was proud of these and felt so pretty wearing them 🩷</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kets4s5xh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1gxel25</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Length difference 🤣</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae5arbrswh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1gxe8tv</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Is it too soon for a fill?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsi481m9uh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1gxe42d</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>My first set of nails to give to a family friend! What do you think?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0g33xzath2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1gxdy0g</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Any recommendations for broken nails ?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdy0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1gxdmzn</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>The horror and the redemption.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdmzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1gxdavp</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>turning old nails into sets for practice! (swipe for before, still fighting with my chrome until my new lamp arrives).</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdavp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1gxcj5l</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye nails </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoz5f85rhh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1gxbo82</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>should i ask for a refund?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlzxima6bh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1gxb109</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Tips on acrylics?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gxb109/tips_on_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1gxbbcu</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>🧡 Disney Halloween Nails 🧡</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9px6dij8h2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1gxazav</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Novice guy here</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jbiow726h2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1gxavbr</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Love my nail girl nailsbysavannah</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxavbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1gx4487</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Persistently Cracked Cuticles. Help!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gx4487/persistently_cracked_cuticles_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1gx22ay</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>My first pre decorated Gel X set</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyzkrub4je2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1gwxecq</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>DND gel sale</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gwxecq/dnd_gel_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1gxabu5</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>What color should I do next?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sbrf34y0h2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1gxa838</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Oh the weather outside is frightful… ❄️</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxa838</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1gxa3o1</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Eras Tour nails for tonight ✨ </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxa3o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1gx9yk3</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I’m Obsessed.</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z07sx44yg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1gx9va4</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Fresh nails</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn0tgxfcxg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1gx9p98</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red is such a baddie color </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx9p98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1gx9kgp</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Who else never does any color on their toenails apart from white?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmeuuymxug2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1gx980j</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Do You like this design?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0q01pe42sg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1gx95c0</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In my press on nails era </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0d1pu6frg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1gx8yg0</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I love color</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmauminupg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1gx8u7u</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Did some basic but cute nails for winter season 😅 Too much or okay to go with?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9hkr7rpog2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1gx7i9r</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47964k15dg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1gx70jt</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>new nails, natural ❤️</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/havbet4p8g2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1gx6upx</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Just need some advice -- can you decide if gel or acrylic is right for me?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gx6upx/just_need_some_advice_can_you_decide_if_gel_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1gx6ta4</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>My 6-year-old’s press ons</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7ct3ubn6g2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1gx5z4v</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>It's such an unusual color for me, but I love it</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqg6w4gsxf2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1gx5h5u</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>UV green on black</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrq2wga0sf2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1gx50cs</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>My mindblowing nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx50cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1gx4tti</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I'm blown away by ILNP's 'Hi-Fi'!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2aqkeyzjf2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1gx497k</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Glinda/witchy nail shape for movie night</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6rw54svhcf2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1gx45p6</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Is my UV lamp rubbish or am I doing it wrong?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gx45p6/is_my_uv_lamp_rubbish_or_am_i_doing_it_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1gx32j9</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>The Fall Set 🧡🍂</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx32j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1gxujwz</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Ignoring the finish here, what nail polish is closest to the base color shown?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a4ewea8xl2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1gxt7ya</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a thermal that captures these vampy sangria tones?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkpqp8vlgl2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1gxsuva</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ORLY Lost Treasure </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk30l26fcl2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1gxs0jp</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>{PR} Meet “Eccentric” by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxs0jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1gxr353</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Shade question</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yoc9ss9dtk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1gxqztj</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>If you've bought peacci polish, how accurate are the web site images/video to what you received?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxqztj/if_youve_bought_peacci_polish_how_accurate_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1gxqit1</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Purple gift wrap!</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10mq5zrqnk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1gxq66r</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Magnetic Polish Swatches</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxq66r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1gxpj10</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Cold As Ice matches my ring!</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyrbyguwdk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1gxp7sb</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rogue Lacquer’a Black Friday sale just started! Here’s my order! All the shifties! </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp7c1k8xak2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1gxp5xn</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nails over 1 inch </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxp5xn/which_nails_over_1_inch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1gxok7h</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>If you could only shop one Black Friday sale…</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxok7h/if_you_could_only_shop_one_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1gxo4lf</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Synchrony 💛💚🩵</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxo4lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1gxo0d5</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Badgers! Flowers!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxo0d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1gxny4w</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can y'all help me find a shade very close to  this? </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw4q3gcazj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1gxnq81</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>"Full scream ahead" featuring a jumping spider!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxnq81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1gxnls8</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Glowy goodness</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74ws48d8wj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1gxmmtp</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Amy by Zoya</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5cvnsvynj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1gxmeau</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know the shade of Dorits nail polish in this scene? </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnvv3z8bbj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1gxmbnz</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Accidentally found this insane emerald for Wicked nails</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxmbnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1gxl4yk</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boutique and Indie polish </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxl4yk/boutique_and_indie_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1gxkq0h</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Apparently I telepathically picked up on the weekend’s mani trend this morning</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4zgf37h8j2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1gxkkbn</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Blister on hyponychium?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76pd5rd97j2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1gxka0c</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long Distance Relationship </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwocad1x4j2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1gxk8lf</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I like sheers over solids </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxk8lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1gxjqkh</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Getting in the Wicked Train For The Weekend</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pq0cl8f0j2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1gxjcvg</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Slots of Fun is UNREAL</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxjcvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1gxiuzh</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>KB Shimmer shipping cost?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxiuzh/kb_shimmer_shipping_cost/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1gxiokl</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Zoya Black Friday</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxiokl/zoya_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1gxik4d</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Greens 💚</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxik4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1gxijth</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>So Pretty</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y0z24go5ri2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1gxicoc</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you organize your lacquers? </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxicoc/how_do_you_organize_your_lacquers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1gxi62b</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>I cant decide which to use!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxi62b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1gxi3qx</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosty/Snowy obsession </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxi3qx/frostysnowy_obsession/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1gxhs2e</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Is my whole fingernail crooked or am I filing it lopsided?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxhs2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1gxhrri</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>You guys think if I tweak it a bit I can get this to “read” as gold cobblestones?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i51kgf60li2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1gxhr30</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is just to say how much I appreciate you all so much, &amp; to thank you for never letting me down when I have nail care, or polish/dupe/colours questions! </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u34nqx3vki2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1gxhqn8</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>When you realize you’ve been around awhile 😳💅</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxhqn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1gxhn83</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Saving favorites on Madam Glam website?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxhn83/saving_favorites_on_madam_glam_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1gxhkgu</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>pistachio and raspberry mani to brighten up dreary fall days</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxhkgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1gxhfp9</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Shimmer Showoff 💚</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxhfp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1gxhck5</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Essie Wicked 249 (vintage) Vs. Essie Wicked 352</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxhck5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1gxh73x</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready/Not Ready for Arcane S2 Act 3 to drop tomorrow. </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxh73x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1gxgr6s</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Why don’t nail polish thinners contain isopropyl alcohol?</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxgr6s/why_dont_nail_polish_thinners_contain_isopropyl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1gxgi1y</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Really loving my holiday nails!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k64bgedabi2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1gxgcut</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Comparison Dam Dark Eyed Blossom and Penelope Luz Disco Fever?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxgcut/comparison_dam_dark_eyed_blossom_and_penelope_luz/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1gxfwar</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>I have a confession to make…</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szpsyt7n6i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1gxftv9</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Christmas mismatch set!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxftv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1gxfikm</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Desperately searching for a dupe! Bought this gorgeous rusty, reddish, earthy red in France 5 years ago and need a new bottle please  </t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3faxwbks3i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1gxfii4</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked mani. </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxfii4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1gxf6pf</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Megan’s mini mani</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxf6pf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1gxeq6v</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Cuticle Products</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxeq6v/cuticle_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1gxemw5</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Does anyone have comparison swatches for MC Shroomdom and HT Favorite Sister?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxemw5/does_anyone_have_comparison_swatches_for_mc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1gxe8cy</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>I’m almost out of one of my favorite polishes and need a dupe: Illimite La Femme Fleur, discontinued :( thanks!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3b9vvx5uh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1gxe4p8</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Swatch Request - ILNP Black Orchid vs. Dakota vs. Broadway</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxe4p8/swatch_request_ilnp_black_orchid_vs_dakota_vs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1gxe3z4</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>💅 Swatching the Digital Dystopia Collection by Prism Parade - Available Now! [paid pr]</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://youtube.com/watch?v=ZsV-b1EolYw&amp;si=WiAipsOBNc9ylToV</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1gxe10l</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A-England 👑 </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lvd7h9psh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1gxdt2d</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Love this color combo!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdt2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1gxdruk</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Bawwwk bawk bawk</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdruk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1gxdrnb</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>HoloTaco Shadow Lake</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdrnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1gxdn13</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Sapphire</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxdn13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1gxdino</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Break Between Press-On Nails?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxdino/break_between_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1gxdezr</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Mooncat Speed Demon drying issues?</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hlzskm98oh2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1gxdcae</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Loving this color</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s07emxdonh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1gxd6y1</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer addressing the site issues </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ztkw6q6lmh2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1gxch2x</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried to do a fall themed skittle and idk how I feel about it. </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxch2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1gxcd3e</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Does anyone know of a periwinkle shimmer like this one?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxcd3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1gxccap</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>More adventures in magnets!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gwp9qf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1gxca4b</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Cirque Colors “Robin”</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpax8hesfh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1gxbxb9</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can’t decide whether I like these. </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxbxb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1gxbx4s</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It snowed in MN, but Thanksgiving still deserves attention. </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lolhvs81dh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1gxbv6s</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brands NEED to scale their websites for Black Friday </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxbv6s/brands_need_to_scale_their_websites_for_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1gxbu3z</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>kbshimmer website slow?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxbu3z/kbshimmer_website_slow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1gxbtzy</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to? </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k1gqtodch2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1gxbn94</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Seasonally appropriate holo 🤎</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdzsccyyah2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1gxb91y</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Flowers and Cherries</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxb91y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1gxax2i</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>KBShimmer Website</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxax2i/kbshimmer_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1gxam48</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">looking for a nude like in the picture below! any suggestions? </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jekjvvn73h2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1gxaivf</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Court Color?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxaivf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1gx9cdx</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Starrily Black Friday Sale?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gx9cdx/starrily_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1gx82hr</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">User error </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx82hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1gx7z7n</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Does anyone know if Beautometry has a black Friday sale?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gx7z7n/does_anyone_know_if_beautometry_has_a_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1gx7v18</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">China Glaze Ruby Slippers </t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx7v18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1gx7t6a</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Staining or Orangies(is that a thing?)?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vai83ultfg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1gx7bv2</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>ILNP toppers?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj736mkkbg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1gx6syo</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Your heart's a black hole (unmagnetized) 🥀</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx6syo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1gwy6yb</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Is NOL Dream or FG Blue Skies any brighter than SH Miami Ice?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gwy6yb/is_nol_dream_or_fg_blue_skies_any_brighter_than/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1gx4ya2</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In-store vs online polish purchases? </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gx4ya2/instore_vs_online_polish_purchases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1gx666s</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Nails by me myself</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx666s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1gx5fsg</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>ILNP - Dreamscape</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx5fsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1gx444f</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Light up my world</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gx444f/light_up_my_world/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1gx3wb0</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black Friday purchases! </t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cve7yf7q7f2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1gxtunh</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Help me find this creator please!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gxtunh/help_me_find_this_creator_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1gxt7uv</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Pink Bling Set 🩷🤍</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxt7uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1gxqkt9</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Practicing Handpainted nail art </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxqkt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1gxq9vx</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Animal prints</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umoansi9lk2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1gxpze4</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>🍓 Miffy Nails  🍓</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxpze4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1gxnprb</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Animal Crossing Set</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyo35tp7xj2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1gxkjsh</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nails are we getting next? </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gxkjsh/what_nails_are_we_getting_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1gxikw1</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Autumn boho set - matched mani pedi</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxikw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1gxhc2b</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>May Christmas come</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mswubanhi2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1gxg7lq</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Van Gogh Nails 💙✨️</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxg7lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1gxfq7c</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Nail Planning</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnhe8mad5i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1gxfc1w</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>These were supposed to be a “pink Christmas” set but I got carried away 😆</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ws0oxafg2i2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1gxf826</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>How to recreate this set?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxf826</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1gxcysx</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>I’m dreading doing my right hand 🥲</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s9sh4lvkh2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1gxbapl</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>🧡 Disney Halloween Nails 🧡</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5cqi7le8h2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1gx97hp</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inverse heart stiletto nails </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbaelfryrg2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1gx84ne</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">made by @ margg.nails
+</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmy1duwlig2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1gx6ze6</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Opinions pls🙏🏽</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx6ze6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1gx65al</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Nail Art Newbie</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx65al</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1gx4rvy</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been doing a ton of nail art lately! </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx4rvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1gx4r9z</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Finally got around to finishing the whole Grinch set 🎄</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt8vls64jf2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1gx3kab</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday Nails! </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gx3kab</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Nov 24 08:09:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_24.xlsx
+++ b/data/collected_data/2024_11_24.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1203"/>
+  <dimension ref="A1:C1372"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20885,6 +20885,2879 @@
         </is>
       </c>
     </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1gym01u</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glass nail rec? </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gym01u/glass_nail_rec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1gylpvu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>My girlfriend recently started selling her nails! Heres some of her recent work :)</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gylpvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1gylnl2</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel x beginner question </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gylnl2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1gyl7xh</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Was thinking about getting my nails done by this girl, but are these bad?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7n5j25aus2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1gyl664</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">did my sister's nails :) </t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyl664</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1gyktcl</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Hybrid UV/LED lamps (I have questions below 👇🏻)</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyktcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1gyju35</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Fingertip Cut from Salon</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4s5n4fotds2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1gyiurv</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do I keep my nails from lifting </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdp2fk123s2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1gyj9fs</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Should I get a refund for this gel manicure? I literally bled... (Quinns Nails in Kelowna BC)</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyj9fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1gyjswv</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Purple snow naiks</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyjswv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1gyjea3</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>gave myself some jinx nails from arcane</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07xqklpv8s2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1gyj68n</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3s3wid0k6s2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1gyiinb</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Too wide? </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyiinb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1gyhs5o</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>I cannot get these nails off!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gyhs5o/i_cannot_get_these_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1gyhif9</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I loved the color and how delicate they were</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyavq3l6pr2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1gyhhdl</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>simple and subtle winter nails I got! how do we feel about them?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8agvhpvor2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1gyhg8c</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Why is one side of my nail on my middle finger so much weaker than the other side of that same nail?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyhg8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1gyhb6t</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these as bad as I think they are? 😭 </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyhb6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1gyhap3</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Thanksgiving Mani</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/shpayq4zmr2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1gyh9lf</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>New Winter Nails - Studio</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6psta9qmr2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1gygppv</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice Nails </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22lbqe3ahr2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1gygoae</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>pictures don't really do it justice 🦪🫧🦢🪩</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gygoae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1gygeov</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gygeov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1gyg9qv</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Gel-X + Cat Eye Practice!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyg9qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1gyg2xu</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>pink nail salon lotion?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gyg2xu/pink_nail_salon_lotion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1gyfwpm</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new favorite nails! </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ps6pxaon9r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1gyfvc1</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>black and red 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g12ziqma9r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1gyfivr</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Recommendations for really hard/sturdy press-ons?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e5xwd966r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1gyfitn</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Some festive green and gold</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1gzv5o56r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1gyf4b7</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">goth gworl nails </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgiqe3hg2r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1gyf2df</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish recommendations </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gyf2df/polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1gyeejz</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the best nail shape ? </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyeejz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1gydvbi</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple copper dots </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68hbfdtkrq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1gycw2y</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5od1h78jq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1gydj99</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech killed it and fulfilled my Sukuna obsession 🫶🏼😤✨ s/o to all the anime lovers who help create special sets like these ♥️ </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gydj99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1gycn1o</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>My 1930's inspired half moon nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gycn1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1gybtba</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail set i did myself today! </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf19fqacaq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1gy5yop</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>how do i remove the rest of acrylics?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gy5yop/how_do_i_remove_the_rest_of_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1gybkzy</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Kiss Press on nails and kids</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gybkzy/kiss_press_on_nails_and_kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1gyauhu</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Blow me up with ideas for my next nail color!</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gyauhu/blow_me_up_with_ideas_for_my_next_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1gy9ufk</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cm78e36jup2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1gy9s16</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails I'm about to remove </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yhscqdpztp2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1gy7n60</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Good no wipe top coat?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gy7n60/good_no_wipe_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1gyaifj</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>DIY Chocolatey nails for fall 🤎</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2su2zstzp2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1gyaepk</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Press ons🔮</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyaepk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1gya1hr</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mom let me give her some acrylics 😀 </t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25tqbi03wp2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1gy9qzo</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Having a hard time removing MMA acrylic</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gy9qzo/having_a_hard_time_removing_mma_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1gy9ndo</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best set I've done in myself thus far </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqhezbqzsp2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1gy9k0b</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festive 🎄 </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j93jdot9sp2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1gy9hik</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbed wire nails </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9tgxo9qrp2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1gy9exo</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Molten Sky is beautiful ❤️💜🤎</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy9exo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1gy9bl7</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Nails dented and curling?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy9bl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1gy8hwz</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Growing out my 'i hate pink' phase</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy8hwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1gy6yef</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reindeer Nails for Christmas </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lamomxor7p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1gy6vul</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>I love pink colour</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56fgq4z77p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1gy6k4j</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>brown for fall… groundbreaking</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xy0d3zq4p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1gy6fpe</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>MANicures!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy6fpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1gy6epr</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Red Cateyes ❤️</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy6epr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1gy630b</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>my fall teddy bear nails 🧸🤎</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyi5f5u21p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1gy60os</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>🍁</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o25ayw8l0p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1gy514t</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>If I can’t have exaggerated nails then my dangly charms will have to do</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyg7o0ryso2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1gy4t54</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>miss my august nails 💖</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73d9nhrzqo2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1gy4n5f</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is my nail shape? </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy4n5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1gy3vzv</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy3vzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1gy387v</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Fancy green beauties</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy387v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1gy2xmq</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My duck nails 😁 Enyway i love them 😍</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy2xmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1gy2aky</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>I tried magnetic😁</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy2aky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1gy1ts2</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>🎀Festive Bows 🎀</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3lgton04o2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1gy1l9w</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>❄️ Winter Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/josoco842o2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1gy1bfv</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another blue? Oh, go on then </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy1bfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1gy1axk</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Please recommend a nice nail polish gift (set), I don't know where to start and want to gift someone who is into doing their nails! 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gy1axk/please_recommend_a_nice_nail_polish_gift_set_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1gy0u44</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>We used stickers, color gel and imagination. 🎉🧚</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy0u44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1gy00uk</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Shabby chic raised set</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd2djstqon2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1gxzsba</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Did my own nails at a friend's place last night ✨</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxzsba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1gxyenr</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>The second time I did my own nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv8qx4bp8n2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1gxxwc3</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Black Swan</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxxwc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1gxwgeh</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Cherry red for December🍒</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixqt7dlklm2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1gxvukd</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>💙🩷</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxvukd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1gyl1l8</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Teal Glitter Gel Pen!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyl1l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1gyk1h1</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">best for newbies!? I'm a hardcore gel polish user but it just eats up too much of my life, what are your favorite base and top coats for those that are in the beginning stages of that transition? i love the gel look.. something that levels out your nail and has long term shine! </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyk1h1/best_for_newbies_im_a_hardcore_gel_polish_user/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1gyjzbc</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Does anyone use IKEA Kallax w/ drawers for polish storage?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyjzbc/does_anyone_use_ikea_kallax_w_drawers_for_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1gyjhg7</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Can I get some opi recommendations for these colors? Only looking for opi as it lasts the longest on me. Also looking for opaque with 2 coats. My skintone is similar to the ones in photos 2,4,5.</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyjhg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1gyin13</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>More November nails</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyin13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1gyi5ei</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Norpsilocin by Clionadh</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/icu6xhdovr2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1gyhq19</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best undies for sheer polish? Cirque jellies or polished for days base coat? </t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyhq19/best_undies_for_sheer_polish_cirque_jellies_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1gyh4fu</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>My first Polish Pickup</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4i7f8oclr2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1gygs2v</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>My Wicked Nails</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gygs2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1gygjvj</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Molten Sky is beautiful ❤️💜🤎</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy9exo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1gygh5h</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked stamping! </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gygh5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1gygd0x</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Many Faces of Wizard Duel Chrome </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gygd0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1gyfrwl</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Mesmerized with LynB</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64t5rrff8r2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1gyfky4</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer: Trick or Treat Yourself</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyfky4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1gyfj4o</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a good black gel polish </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyfj4o/looking_for_a_good_black_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1gyfh4g</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Holding Paws 🐶</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyfh4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1gyfb9l</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Cleanliness and nail growth?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyfb9l/cleanliness_and_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1gyf6fz</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>birthday nails!! (reupload)</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyf6fz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1gyesvm</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Emo + OPI Awe Night Long</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyesvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1gyef1r</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>She’s a shiftyyyy bish!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyef1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1gyednt</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Mooncat - Smokescreen!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dp38yn8yvq2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1gyedm8</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple Agate - yet another that photographs don't capture the beauty of! </t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyedm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1gye1um</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Marble effect!</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gye1um</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1gydwqy</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>I love this stuff, but hate the scent. Any similar lotions?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90053iixrq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1gydpoe</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first thermal </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5whbq98qq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1gyd7st</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Swatch Request - Sally Hansen Once Upon a Holiday Collection</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdb8y9l0mq2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1gyc9cq</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️🧲</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fia1f722eq2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1gyc5mr</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Tips for french tips?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyc5mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1gybh7l</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Harlow &amp; Co and Canada Post Strike</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gybh7l/harlow_co_and_canada_post_strike/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1gyb0sh</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>I wanted to see Dark Horse and Stop the Clock side by side 🤎🟤</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc9auanz3q2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1gyasan</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Sweet combo</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qz4wi3d02q2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1gyahj1</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Freshly velvetized After Hours</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d9pwfb9lzp2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1gyafwh</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Help me pick an ILNP polish outside of my comfort zone?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gyafwh/help_me_pick_an_ilnp_polish_outside_of_my_comfort/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1gy9uab</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to avoid skin staining when removing strong/dark colours? </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9e79mqiup2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1gy9or0</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>I couldn’t resist doing a full manicure of the magnetic squiggles 〰️</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy9or0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1gy94db</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI Wicked line still holding strong 1 week later but I think my dog is getting sick of me using her paw to show off my nails </t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp2xm93sop2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1gy93ol</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Recommendations for green polish w/ red or pink shimmer</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy93ol/recommendations_for_green_polish_w_red_or_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1gy8gjr</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Tops for getting glue off the surface of press ons?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6yv8vxijp2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1gy8a00</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Black Friday?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy8a00/dazzle_dry_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1gy891c</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WHY 😭 </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g93qh7rhp2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1gy83ly</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>first snow means champagne nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy83ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1gy7yoy</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Happy Thanksgiving, Laqueristas!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy7yoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1gy7u95</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sitting here creating wishlists  </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivz6sazlep2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1gy79hp</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love magnetic multichromes </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy79hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1gy781u</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>First dupes in my collection</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy781u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1gy6oxz</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>ILNP - Ariel 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uec6umq5p2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1gy6fi5</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Red Cateyes❤️</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy6fi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1gy5raz</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Advice on gel polish for a beginner.</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy5raz/advice_on_gel_polish_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1gy64qq</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Ethereal - Black Cat Mystery Polish - Meow (magnetic)</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy64qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1gy5wz4</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Tried some cool nail art and stickers 🕷️🥀</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy5wz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1gy5og4</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Serenity by ILNP</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dzweinvxxo2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1gy5asx</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>🥜PB&amp;J Watermarble🥜</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy5asx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1gy59as</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Black Friday MADDNESS</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt2whfqquo2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1gy58dw</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Picked up my engagement ring today and needed a matching nail polish…</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxlfl5rjuo2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1gy51bw</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Kbshimmer shipping?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy51bw/kbshimmer_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1gy4nwn</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Black Opal inspired by BlackOpalDirect</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy4nwn/black_opal_inspired_by_blackopaldirect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1gy4i82</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>🤩 Clionadh- Norpsilocin</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kw226lovoo2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1gy4hrj</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Me trying to convince myself not to pick at a hangnail.</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgk5ml4soo2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1gy46rr</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Can anyone compare Cobalt Dreams by Emily de Molly for me to other comparables?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy46rr/can_anyone_compare_cobalt_dreams_by_emily_de/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1gy43ql</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>What are we doing for toe colors?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy43ql/what_are_we_doing_for_toe_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1gy30vw</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Frozen Bubbles over Missed Shift</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy30vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1gy2qqq</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Zero Degrees vs VIP Swatches? </t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>/r/ILNP/comments/1gxzzhn/zero_degrees_vs_vip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1gy2mne</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Finally figured out chrome nails!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy2mne</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1gy1xqx</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Autumn Leaves 🍂</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k9h28vv4o2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1gy1oyw</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>❄️✨</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwkp2qpy2o2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1gy1niw</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At 4am my partner shifted in bed and my pinky was in the wrong place at the wrong time 😭 </t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd3iyrkm2o2e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1gy1a4o</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Huge Shoutout to Glisten and Glow!!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dtrvymkzn2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1gy11qy</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Silk wrap recommendations</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy11qy/silk_wrap_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1gy09t2</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Organizing your polish </t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy09t2/organizing_your_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1gy03dd</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coat on press ons </t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gy03dd/top_coat_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1gxzl9f</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi wicked </t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxzl9f/opi_wicked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1gxy0rm</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Black Swan</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxy0rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1gxwe2r</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found this gem in my old polish collection from wayy back when </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxwe2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1gxjdwj</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>My first time trying Sassy Sauce!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i75e2mlpxi2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1gxk2n8</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Gel-like top coat without shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gxk2n8/gellike_top_coat_without_shrinkage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1gxm1eq</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Underglow Skittle</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxm1eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1gxuwrj</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Velvet magnetic help</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxuwrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1gylp3h</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>My girlfriend recently started selling her nails! Here is some of her recent work :)</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gylp3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1gygi0w</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Ideas for fun but professional nails</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gygi0w/ideas_for_fun_but_professional_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1gyfhoh</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>16 Wishes ✨️🧚‍♀️💞 i'm halfway done but wanted to share anyway 💕 I always loved this movie so when I saw someone else make a set last night, I immediately had to make my own!</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gyfhoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1gydrc9</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Christmas set 💚😍💅🏼</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mlau16wkqq2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1gya6aa</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Thanksgiving Pressons</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gya6aa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1gy9std</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>My current set</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0gmn2of6up2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1gy8b7m</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>🔥 🩸Bday Nails for a friend 🩸🔥</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy8b7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1gy70wu</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Tortoise shell help</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy70wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1gy6guz</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Red Cateye Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy6guz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1gy5zic</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Tried some cool nail art and stickers 🕷️🥀</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy5zic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1gy24si</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Winter Nails!! (With and without filter)</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gy24si</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1gy1kxk</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>❄️ Winter Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tthn6n712o2e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1gxzwj8</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much is this set?? </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j2kxz5cnnn2e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1gxuubr</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Vintage-inspired watercolor Christmas nails I finished a couple days ago ✨️</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gxuubr</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>